<commit_message>
optimized code + time checks for functions
For tmfcenter.com performance imporved by 64% from 79 seconds to just 28 seconds
</commit_message>
<xml_diff>
--- a/batchwise_companies.xlsx
+++ b/batchwise_companies.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DCMME_git\Web-scrapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CD6715-A195-48FF-BFC7-38410DF3C410}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321ED7B8-8DE4-4A19-A319-B65F81EE464A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9402" firstSheet="4" activeTab="17" xr2:uid="{3BB731C8-CC94-416A-9520-170C1B6F9CC4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9402" activeTab="1" xr2:uid="{3BB731C8-CC94-416A-9520-170C1B6F9CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="batch1" sheetId="1" r:id="rId1"/>
-    <sheet name="batch2 " sheetId="2" r:id="rId2"/>
+    <sheet name="batch2" sheetId="2" r:id="rId2"/>
     <sheet name="batch3" sheetId="3" r:id="rId3"/>
     <sheet name="batch4" sheetId="4" r:id="rId4"/>
     <sheet name="batch5" sheetId="5" r:id="rId5"/>
@@ -8000,7 +8000,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9310,7 +9310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402187A4-2E61-4484-8367-EA5878C59535}">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -9611,7 +9611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28316556-7D01-4CB9-8F25-963CF760623D}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -13530,9 +13530,9 @@
     <cfRule type="duplicateValues" dxfId="33" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="32" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="31" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
     <cfRule type="duplicateValues" dxfId="29" priority="9"/>

</xml_diff>